<commit_message>
feat: last prj files
</commit_message>
<xml_diff>
--- a/PRJ-23/Otimização/Resultados/Potimizacao.xlsx
+++ b/PRJ-23/Otimização/Resultados/Potimizacao.xlsx
@@ -516,13 +516,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.47</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>2.470000059604645</v>
+        <v>3.000000059604645</v>
       </c>
       <c r="D8">
-        <v>2.41314351317371E-06</v>
+        <v>1.986821492513021E-06</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>